<commit_message>
Added OOI bar codes and SN where needed
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP03ISSP_00004.xlsx
+++ b/deployment/Omaha_Cal_Info_CP03ISSP_00004.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9120" yWindow="1640" windowWidth="27160" windowHeight="16560" tabRatio="579"/>
+    <workbookView xWindow="9120" yWindow="1635" windowWidth="27165" windowHeight="16560" tabRatio="579" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -19,7 +24,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="112">
   <si>
     <t>Ref Des</t>
   </si>
@@ -336,17 +341,47 @@
   <si>
     <t>[ -0.31961300,  -0.22285200,  -0.13591200,  -0.05967300,   0.01131300,   0.06951000,   0.12143700,   0.17570200,   0.22378300,   0.26898300,   0.31277900,   0.35029800,   0.38927900,   0.42159400,   0.45286800,   0.47889900,   0.50785600,   0.53244800,   0.55535100,   0.57890500,   0.60055800,   0.62152200,   0.64165900,   0.66038500,   0.67526900,   0.69040900,   0.70248800,   0.71550500,   0.72701700,   0.73966800,   0.74947800,   0.75869500,   0.76812300,   0.77849000,   0.78779700,   0.79684000,   0.80519000,   0.81263700,   0.81840000,   0.82154700,   0.82229600,   0.81113800,   0.80273300,   0.78799400,   0.76903100,   0.74457700,   0.72625600,   0.71776700,   0.71583600,   0.71779000,   0.71971400,   0.72208000,   0.72334100,   0.72452700,   0.72360600,   0.72069000,   0.71514900,   0.70127800,   0.69316800,   0.68562100,   0.68107800,   0.67899600,   0.67410000,   0.66254400,   0.64540200,   0.61738500,   0.57959600,   0.52837500,   0.46161400,   0.37469500,   0.26502200,   0.12878300,  -0.04182300,  -0.24088100,  -0.47724100,  -0.73282700,  -0.97133400,  -1.17354500,  -1.30832900,  -1.38777300]</t>
   </si>
+  <si>
+    <t>OL000269</t>
+  </si>
+  <si>
+    <t>N00564</t>
+  </si>
+  <si>
+    <t>N00565</t>
+  </si>
+  <si>
+    <t>OL000270</t>
+  </si>
+  <si>
+    <t>N00567</t>
+  </si>
+  <si>
+    <t>N00568</t>
+  </si>
+  <si>
+    <t>N00569</t>
+  </si>
+  <si>
+    <t>N00570</t>
+  </si>
+  <si>
+    <t>N00571</t>
+  </si>
+  <si>
+    <t>N00124</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="168" formatCode="0.000E+00"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="33" x14ac:knownFonts="1">
     <font>
@@ -652,14 +687,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -1249,7 +1284,7 @@
     <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1273,10 +1308,10 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1299,7 +1334,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1344,7 +1379,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1934,7 +1969,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Moorings"/>
@@ -2274,28 +2309,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="34.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" customWidth="1"/>
-    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="34.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="11" customFormat="1" ht="28">
+    <row r="1" spans="1:14" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>83</v>
       </c>
@@ -2334,8 +2369,10 @@
       </c>
       <c r="M1" s="34"/>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="29"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
       <c r="B2" s="29" t="s">
         <v>64</v>
       </c>
@@ -2372,20 +2409,20 @@
       </c>
       <c r="N2" s="14"/>
     </row>
-    <row r="3" spans="1:14" s="18" customFormat="1">
+    <row r="3" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="19"/>
       <c r="E3" s="20"/>
       <c r="F3" s="21"/>
       <c r="G3" s="20"/>
       <c r="H3" s="29"/>
     </row>
-    <row r="4" spans="1:14" s="18" customFormat="1">
+    <row r="4" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
       <c r="F4" s="21"/>
       <c r="G4" s="20"/>
     </row>
-    <row r="5" spans="1:14" s="18" customFormat="1">
+    <row r="5" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
       <c r="F5" s="21"/>
@@ -2393,73 +2430,73 @@
       <c r="H5" s="27"/>
       <c r="I5" s="27"/>
     </row>
-    <row r="6" spans="1:14" s="18" customFormat="1">
+    <row r="6" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
       <c r="F6" s="21"/>
       <c r="G6" s="20"/>
     </row>
-    <row r="7" spans="1:14" s="18" customFormat="1">
+    <row r="7" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
       <c r="F7" s="21"/>
       <c r="G7" s="20"/>
     </row>
-    <row r="8" spans="1:14" s="18" customFormat="1">
+    <row r="8" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D8" s="19"/>
       <c r="E8" s="20"/>
       <c r="F8" s="21"/>
       <c r="G8" s="20"/>
     </row>
-    <row r="9" spans="1:14" s="18" customFormat="1">
+    <row r="9" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D9" s="19"/>
       <c r="E9" s="20"/>
       <c r="F9" s="21"/>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="1:14" s="18" customFormat="1">
+    <row r="10" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="1:14" s="18" customFormat="1">
+    <row r="11" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
       <c r="F11" s="21"/>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="1:14" s="18" customFormat="1">
+    <row r="12" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
       <c r="F12" s="21"/>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="1:14" s="18" customFormat="1">
+    <row r="13" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
       <c r="F13" s="21"/>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="1:14" s="18" customFormat="1">
+    <row r="14" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
       <c r="F14" s="21"/>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="1:14" s="18" customFormat="1">
+    <row r="15" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
       <c r="F15" s="21"/>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="1:14" s="18" customFormat="1">
+    <row r="16" spans="1:14" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D16" s="19"/>
       <c r="E16" s="20"/>
       <c r="F16" s="21"/>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="4:7" s="18" customFormat="1">
+    <row r="17" spans="4:7" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D17" s="19"/>
       <c r="E17" s="20"/>
       <c r="F17" s="21"/>
@@ -2478,25 +2515,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N78"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.6640625" customWidth="1"/>
-    <col min="8" max="8" width="57.33203125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="41" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="33" style="12" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2525,21 +2562,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" s="12" customFormat="1">
+    <row r="3" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
       <c r="C3" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D3" s="38">
         <v>4</v>
       </c>
-      <c r="E3" s="40"/>
+      <c r="E3" t="s">
+        <v>103</v>
+      </c>
       <c r="F3" s="40">
         <v>350</v>
       </c>
@@ -2553,18 +2594,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="12" customFormat="1">
+    <row r="4" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B4"/>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
       <c r="C4" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D4" s="38">
         <v>4</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" t="s">
+        <v>103</v>
+      </c>
       <c r="F4" s="40">
         <v>350</v>
       </c>
@@ -2578,18 +2623,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="12" customFormat="1">
+    <row r="5" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
       <c r="C5" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D5" s="38">
         <v>4</v>
       </c>
-      <c r="E5" s="40"/>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
       <c r="F5" s="40">
         <v>350</v>
       </c>
@@ -2603,18 +2652,22 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="12" customFormat="1">
+    <row r="6" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
       <c r="C6" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D6" s="38">
         <v>4</v>
       </c>
-      <c r="E6" s="40"/>
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
       <c r="F6" s="40">
         <v>350</v>
       </c>
@@ -2625,7 +2678,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="12" customFormat="1">
+    <row r="7" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="39"/>
@@ -2634,18 +2687,22 @@
       <c r="F7" s="40"/>
       <c r="H7" s="23"/>
     </row>
-    <row r="8" spans="1:9" s="12" customFormat="1">
+    <row r="8" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
       <c r="C8" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D8" s="38">
         <v>4</v>
       </c>
-      <c r="E8" s="40"/>
+      <c r="E8" t="s">
+        <v>104</v>
+      </c>
       <c r="F8" s="42">
         <v>145</v>
       </c>
@@ -2657,18 +2714,22 @@
       </c>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:9" s="12" customFormat="1">
+    <row r="9" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
       <c r="C9" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D9" s="38">
         <v>4</v>
       </c>
-      <c r="E9" s="40"/>
+      <c r="E9" t="s">
+        <v>104</v>
+      </c>
       <c r="F9" s="42">
         <v>145</v>
       </c>
@@ -2680,18 +2741,22 @@
       </c>
       <c r="I9" s="16"/>
     </row>
-    <row r="10" spans="1:9" s="12" customFormat="1">
+    <row r="10" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
       <c r="C10" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D10" s="38">
         <v>4</v>
       </c>
-      <c r="E10" s="40"/>
+      <c r="E10" t="s">
+        <v>104</v>
+      </c>
       <c r="F10" s="42">
         <v>145</v>
       </c>
@@ -2703,18 +2768,22 @@
       </c>
       <c r="I10" s="16"/>
     </row>
-    <row r="11" spans="1:9" s="12" customFormat="1">
+    <row r="11" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B11"/>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
       <c r="C11" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D11" s="38">
         <v>4</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" t="s">
+        <v>104</v>
+      </c>
       <c r="F11" s="42">
         <v>145</v>
       </c>
@@ -2726,18 +2795,22 @@
       </c>
       <c r="I11" s="16"/>
     </row>
-    <row r="12" spans="1:9" s="12" customFormat="1">
+    <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B12"/>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
       <c r="C12" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D12" s="38">
         <v>4</v>
       </c>
-      <c r="E12" s="40"/>
+      <c r="E12" t="s">
+        <v>104</v>
+      </c>
       <c r="F12" s="42">
         <v>145</v>
       </c>
@@ -2749,18 +2822,22 @@
       </c>
       <c r="I12" s="16"/>
     </row>
-    <row r="13" spans="1:9" s="12" customFormat="1">
+    <row r="13" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B13"/>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
       <c r="C13" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D13" s="38">
         <v>4</v>
       </c>
-      <c r="E13" s="40"/>
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
       <c r="F13" s="42">
         <v>145</v>
       </c>
@@ -2772,18 +2849,22 @@
       </c>
       <c r="I13" s="16"/>
     </row>
-    <row r="14" spans="1:9" s="12" customFormat="1">
+    <row r="14" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B14"/>
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
       <c r="C14" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D14" s="38">
         <v>4</v>
       </c>
-      <c r="E14" s="40"/>
+      <c r="E14" t="s">
+        <v>104</v>
+      </c>
       <c r="F14" s="42">
         <v>145</v>
       </c>
@@ -2795,18 +2876,22 @@
       </c>
       <c r="I14" s="16"/>
     </row>
-    <row r="15" spans="1:9" s="12" customFormat="1">
+    <row r="15" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B15"/>
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
       <c r="C15" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D15" s="38">
         <v>4</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" t="s">
+        <v>104</v>
+      </c>
       <c r="F15" s="42">
         <v>145</v>
       </c>
@@ -2818,7 +2903,7 @@
       </c>
       <c r="I15" s="16"/>
     </row>
-    <row r="16" spans="1:9" s="12" customFormat="1">
+    <row r="16" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="39"/>
@@ -2827,18 +2912,22 @@
       <c r="F16" s="40"/>
       <c r="H16" s="23"/>
     </row>
-    <row r="17" spans="1:14" s="12" customFormat="1">
+    <row r="17" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B17"/>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
       <c r="C17" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D17" s="38">
         <v>4</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" t="s">
+        <v>105</v>
+      </c>
       <c r="F17" s="40" t="s">
         <v>88</v>
       </c>
@@ -2852,18 +2941,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="12" customFormat="1">
+    <row r="18" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B18"/>
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
       <c r="C18" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D18" s="38">
         <v>4</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" t="s">
+        <v>105</v>
+      </c>
       <c r="F18" s="40" t="s">
         <v>88</v>
       </c>
@@ -2877,7 +2970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="12" customFormat="1">
+    <row r="19" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="39"/>
@@ -2886,18 +2979,22 @@
       <c r="F19" s="40"/>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="1:14" s="12" customFormat="1">
+    <row r="20" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B20"/>
+      <c r="B20" t="s">
+        <v>102</v>
+      </c>
       <c r="C20" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="38">
         <v>4</v>
       </c>
-      <c r="E20" s="40"/>
+      <c r="E20" t="s">
+        <v>106</v>
+      </c>
       <c r="F20" s="40">
         <v>427</v>
       </c>
@@ -2911,18 +3008,22 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="12" customFormat="1">
+    <row r="21" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B21"/>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
       <c r="C21" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D21" s="38">
         <v>4</v>
       </c>
-      <c r="E21" s="40"/>
+      <c r="E21" t="s">
+        <v>106</v>
+      </c>
       <c r="F21" s="40">
         <v>427</v>
       </c>
@@ -2936,18 +3037,22 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="12" customFormat="1">
+    <row r="22" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B22"/>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
       <c r="C22" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D22" s="38">
         <v>4</v>
       </c>
-      <c r="E22" s="40"/>
+      <c r="E22" t="s">
+        <v>106</v>
+      </c>
       <c r="F22" s="40">
         <v>427</v>
       </c>
@@ -2961,18 +3066,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="12" customFormat="1">
+    <row r="23" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B23"/>
+      <c r="B23" t="s">
+        <v>102</v>
+      </c>
       <c r="C23" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D23" s="38">
         <v>4</v>
       </c>
-      <c r="E23" s="40"/>
+      <c r="E23" t="s">
+        <v>106</v>
+      </c>
       <c r="F23" s="40">
         <v>427</v>
       </c>
@@ -2986,18 +3095,22 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="12" customFormat="1">
+    <row r="24" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B24"/>
+      <c r="B24" t="s">
+        <v>102</v>
+      </c>
       <c r="C24" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D24" s="38">
         <v>4</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" t="s">
+        <v>106</v>
+      </c>
       <c r="F24" s="40">
         <v>427</v>
       </c>
@@ -3011,18 +3124,22 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="12" customFormat="1">
+    <row r="25" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B25"/>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
       <c r="C25" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="38">
         <v>4</v>
       </c>
-      <c r="E25" s="40"/>
+      <c r="E25" t="s">
+        <v>106</v>
+      </c>
       <c r="F25" s="40">
         <v>427</v>
       </c>
@@ -3035,22 +3152,23 @@
       <c r="I25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="N25" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="12" customFormat="1">
+    </row>
+    <row r="26" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B26"/>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
       <c r="C26" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D26" s="38">
         <v>4</v>
       </c>
-      <c r="E26" s="40"/>
+      <c r="E26" t="s">
+        <v>106</v>
+      </c>
       <c r="F26" s="40">
         <v>427</v>
       </c>
@@ -3063,11 +3181,8 @@
       <c r="I26" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="N26" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" s="12" customFormat="1">
+    </row>
+    <row r="27" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="39"/>
@@ -3075,22 +3190,23 @@
       <c r="E27" s="35"/>
       <c r="F27" s="40"/>
       <c r="H27" s="23"/>
-      <c r="N27" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="12" customFormat="1">
+    </row>
+    <row r="28" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B28"/>
+      <c r="B28" t="s">
+        <v>102</v>
+      </c>
       <c r="C28" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D28" s="38">
         <v>4</v>
       </c>
-      <c r="E28" s="40"/>
+      <c r="E28" t="s">
+        <v>107</v>
+      </c>
       <c r="F28" s="40">
         <v>263</v>
       </c>
@@ -3100,22 +3216,23 @@
       <c r="H28" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="N28" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" s="12" customFormat="1">
+    </row>
+    <row r="29" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B29"/>
+      <c r="B29" t="s">
+        <v>102</v>
+      </c>
       <c r="C29" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D29" s="38">
         <v>4</v>
       </c>
-      <c r="E29" s="40"/>
+      <c r="E29" t="s">
+        <v>107</v>
+      </c>
       <c r="F29" s="40">
         <v>263</v>
       </c>
@@ -3125,22 +3242,23 @@
       <c r="H29" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="N29" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" s="12" customFormat="1">
+    </row>
+    <row r="30" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B30"/>
+      <c r="B30" t="s">
+        <v>102</v>
+      </c>
       <c r="C30" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D30" s="38">
         <v>4</v>
       </c>
-      <c r="E30" s="40"/>
+      <c r="E30" t="s">
+        <v>107</v>
+      </c>
       <c r="F30" s="40">
         <v>263</v>
       </c>
@@ -3150,11 +3268,8 @@
       <c r="H30" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="N30" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" s="12" customFormat="1">
+    </row>
+    <row r="31" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="39"/>
@@ -3162,22 +3277,23 @@
       <c r="E31" s="35"/>
       <c r="F31" s="40"/>
       <c r="H31" s="23"/>
-      <c r="N31" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="12" customFormat="1">
+    </row>
+    <row r="32" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B32"/>
+      <c r="B32" t="s">
+        <v>102</v>
+      </c>
       <c r="C32" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D32" s="38">
         <v>4</v>
       </c>
-      <c r="E32" s="40"/>
+      <c r="E32" t="s">
+        <v>108</v>
+      </c>
       <c r="F32" s="40" t="s">
         <v>89</v>
       </c>
@@ -3190,22 +3306,23 @@
       <c r="I32" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N32" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="12" customFormat="1">
+    </row>
+    <row r="33" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B33"/>
+      <c r="B33" t="s">
+        <v>102</v>
+      </c>
       <c r="C33" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D33" s="38">
         <v>4</v>
       </c>
-      <c r="E33" s="40"/>
+      <c r="E33" t="s">
+        <v>108</v>
+      </c>
       <c r="F33" s="40" t="s">
         <v>89</v>
       </c>
@@ -3219,18 +3336,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="12" customFormat="1">
+    <row r="34" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B34"/>
+      <c r="B34" t="s">
+        <v>102</v>
+      </c>
       <c r="C34" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D34" s="38">
         <v>4</v>
       </c>
-      <c r="E34" s="40"/>
+      <c r="E34" t="s">
+        <v>108</v>
+      </c>
       <c r="F34" s="40" t="s">
         <v>89</v>
       </c>
@@ -3244,18 +3365,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="12" customFormat="1">
+    <row r="35" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B35"/>
+      <c r="B35" t="s">
+        <v>102</v>
+      </c>
       <c r="C35" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D35" s="38">
         <v>4</v>
       </c>
-      <c r="E35" s="40"/>
+      <c r="E35" t="s">
+        <v>108</v>
+      </c>
       <c r="F35" s="40" t="s">
         <v>89</v>
       </c>
@@ -3269,18 +3394,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="12" customFormat="1">
+    <row r="36" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B36"/>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
       <c r="C36" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D36" s="38">
         <v>4</v>
       </c>
-      <c r="E36" s="40"/>
+      <c r="E36" t="s">
+        <v>108</v>
+      </c>
       <c r="F36" s="40" t="s">
         <v>89</v>
       </c>
@@ -3294,18 +3423,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="12" customFormat="1">
+    <row r="37" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B37"/>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
       <c r="C37" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D37" s="38">
         <v>4</v>
       </c>
-      <c r="E37" s="40"/>
+      <c r="E37" t="s">
+        <v>108</v>
+      </c>
       <c r="F37" s="40" t="s">
         <v>89</v>
       </c>
@@ -3319,18 +3452,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="12" customFormat="1">
+    <row r="38" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B38"/>
+      <c r="B38" t="s">
+        <v>102</v>
+      </c>
       <c r="C38" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D38" s="38">
         <v>4</v>
       </c>
-      <c r="E38" s="40"/>
+      <c r="E38" t="s">
+        <v>108</v>
+      </c>
       <c r="F38" s="40" t="s">
         <v>89</v>
       </c>
@@ -3344,18 +3481,22 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="12" customFormat="1">
+    <row r="39" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B39"/>
+      <c r="B39" t="s">
+        <v>102</v>
+      </c>
       <c r="C39" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D39" s="38">
         <v>4</v>
       </c>
-      <c r="E39" s="40"/>
+      <c r="E39" t="s">
+        <v>108</v>
+      </c>
       <c r="F39" s="40" t="s">
         <v>89</v>
       </c>
@@ -3369,18 +3510,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="12" customFormat="1">
+    <row r="40" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B40"/>
+      <c r="B40" t="s">
+        <v>102</v>
+      </c>
       <c r="C40" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D40" s="38">
         <v>4</v>
       </c>
-      <c r="E40" s="40"/>
+      <c r="E40" t="s">
+        <v>108</v>
+      </c>
       <c r="F40" s="40" t="s">
         <v>89</v>
       </c>
@@ -3394,18 +3539,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="12" customFormat="1">
+    <row r="41" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B41"/>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
       <c r="C41" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D41" s="38">
         <v>4</v>
       </c>
-      <c r="E41" s="40"/>
+      <c r="E41" t="s">
+        <v>108</v>
+      </c>
       <c r="F41" s="40" t="s">
         <v>89</v>
       </c>
@@ -3419,7 +3568,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="12" customFormat="1">
+    <row r="42" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="39"/>
@@ -3428,18 +3577,22 @@
       <c r="F42" s="40"/>
       <c r="H42" s="23"/>
     </row>
-    <row r="43" spans="1:9" s="12" customFormat="1">
+    <row r="43" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B43"/>
+      <c r="B43" t="s">
+        <v>102</v>
+      </c>
       <c r="C43" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D43" s="38">
         <v>4</v>
       </c>
-      <c r="E43" s="40"/>
+      <c r="E43" t="s">
+        <v>109</v>
+      </c>
       <c r="F43" s="40" t="s">
         <v>72</v>
       </c>
@@ -3453,18 +3606,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="12" customFormat="1">
+    <row r="44" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B44"/>
+      <c r="B44" t="s">
+        <v>102</v>
+      </c>
       <c r="C44" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D44" s="38">
         <v>4</v>
       </c>
-      <c r="E44" s="40"/>
+      <c r="E44" t="s">
+        <v>109</v>
+      </c>
       <c r="F44" s="40" t="s">
         <v>72</v>
       </c>
@@ -3478,7 +3635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="12" customFormat="1">
+    <row r="45" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="39"/>
@@ -3487,18 +3644,22 @@
       <c r="F45" s="40"/>
       <c r="H45" s="23"/>
     </row>
-    <row r="46" spans="1:9" s="12" customFormat="1">
+    <row r="46" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B46"/>
+      <c r="B46" t="s">
+        <v>102</v>
+      </c>
       <c r="C46" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D46" s="38">
         <v>4</v>
       </c>
-      <c r="E46" s="40"/>
+      <c r="E46" t="s">
+        <v>110</v>
+      </c>
       <c r="F46" s="40">
         <v>407</v>
       </c>
@@ -3509,18 +3670,22 @@
         <v>4439</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="12" customFormat="1">
+    <row r="47" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B47"/>
+      <c r="B47" t="s">
+        <v>102</v>
+      </c>
       <c r="C47" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D47" s="38">
         <v>4</v>
       </c>
-      <c r="E47" s="40"/>
+      <c r="E47" t="s">
+        <v>110</v>
+      </c>
       <c r="F47" s="40">
         <v>407</v>
       </c>
@@ -3531,18 +3696,22 @@
         <v>2826</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="12" customFormat="1">
+    <row r="48" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B48"/>
+      <c r="B48" t="s">
+        <v>102</v>
+      </c>
       <c r="C48" s="39" t="s">
         <v>87</v>
       </c>
       <c r="D48" s="38">
         <v>4</v>
       </c>
-      <c r="E48" s="40"/>
+      <c r="E48" t="s">
+        <v>110</v>
+      </c>
       <c r="F48" s="40">
         <v>407</v>
       </c>
@@ -3553,193 +3722,198 @@
         <v>1.3589</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="22" customFormat="1">
+    <row r="49" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="35"/>
       <c r="D49" s="35"/>
       <c r="E49" s="35"/>
       <c r="F49" s="35"/>
       <c r="H49" s="24"/>
-    </row>
-    <row r="50" spans="1:8" s="12" customFormat="1">
+      <c r="M49" s="12"/>
+    </row>
+    <row r="50" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B50"/>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
       <c r="C50" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D50" s="38">
         <v>4</v>
       </c>
-      <c r="E50" s="40"/>
+      <c r="E50" t="s">
+        <v>111</v>
+      </c>
       <c r="F50" s="43" t="s">
         <v>71</v>
       </c>
       <c r="H50" s="25"/>
     </row>
-    <row r="51" spans="1:8" s="12" customFormat="1">
+    <row r="51" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="40"/>
       <c r="D51" s="40"/>
       <c r="E51" s="37"/>
       <c r="F51" s="37"/>
     </row>
-    <row r="52" spans="1:8" s="12" customFormat="1">
+    <row r="52" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="40"/>
       <c r="D52" s="40"/>
       <c r="E52" s="37"/>
       <c r="F52" s="37"/>
     </row>
-    <row r="53" spans="1:8" s="12" customFormat="1">
+    <row r="53" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="40"/>
       <c r="D53" s="40"/>
       <c r="E53" s="37"/>
       <c r="F53" s="37"/>
     </row>
-    <row r="54" spans="1:8" s="12" customFormat="1">
+    <row r="54" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="40"/>
       <c r="D54" s="40"/>
       <c r="E54" s="37"/>
       <c r="F54" s="37"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C55" s="36"/>
       <c r="D55" s="36"/>
       <c r="E55" s="36"/>
       <c r="F55" s="37"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C56" s="36"/>
       <c r="D56" s="36"/>
       <c r="E56" s="36"/>
       <c r="F56" s="37"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C57" s="36"/>
       <c r="D57" s="36"/>
       <c r="E57" s="36"/>
       <c r="F57" s="37"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C58" s="36"/>
       <c r="D58" s="36"/>
       <c r="E58" s="36"/>
       <c r="F58" s="37"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C59" s="36"/>
       <c r="D59" s="36"/>
       <c r="E59" s="36"/>
       <c r="F59" s="37"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C60" s="36"/>
       <c r="D60" s="36"/>
       <c r="E60" s="36"/>
       <c r="F60" s="37"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C61" s="36"/>
       <c r="D61" s="36"/>
       <c r="E61" s="36"/>
       <c r="F61" s="37"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C62" s="36"/>
       <c r="D62" s="36"/>
       <c r="E62" s="36"/>
       <c r="F62" s="37"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C63" s="36"/>
       <c r="D63" s="36"/>
       <c r="E63" s="36"/>
       <c r="F63" s="37"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C64" s="36"/>
       <c r="D64" s="36"/>
       <c r="E64" s="36"/>
       <c r="F64" s="37"/>
     </row>
-    <row r="65" spans="3:6">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C65" s="36"/>
       <c r="D65" s="36"/>
       <c r="E65" s="36"/>
       <c r="F65" s="37"/>
     </row>
-    <row r="66" spans="3:6">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C66" s="36"/>
       <c r="D66" s="36"/>
       <c r="E66" s="36"/>
       <c r="F66" s="37"/>
     </row>
-    <row r="67" spans="3:6">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C67" s="36"/>
       <c r="D67" s="36"/>
       <c r="E67" s="36"/>
       <c r="F67" s="37"/>
     </row>
-    <row r="68" spans="3:6">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C68" s="36"/>
       <c r="D68" s="36"/>
       <c r="E68" s="36"/>
       <c r="F68" s="37"/>
     </row>
-    <row r="69" spans="3:6">
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C69" s="36"/>
       <c r="D69" s="36"/>
       <c r="E69" s="36"/>
       <c r="F69" s="37"/>
     </row>
-    <row r="70" spans="3:6">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C70" s="36"/>
       <c r="D70" s="36"/>
       <c r="E70" s="36"/>
       <c r="F70" s="37"/>
     </row>
-    <row r="71" spans="3:6">
+    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C71" s="36"/>
       <c r="D71" s="36"/>
       <c r="E71" s="36"/>
       <c r="F71" s="37"/>
     </row>
-    <row r="72" spans="3:6">
+    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C72" s="36"/>
       <c r="D72" s="36"/>
       <c r="E72" s="36"/>
       <c r="F72" s="37"/>
     </row>
-    <row r="73" spans="3:6">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C73" s="36"/>
       <c r="D73" s="36"/>
       <c r="E73" s="36"/>
       <c r="F73" s="37"/>
     </row>
-    <row r="74" spans="3:6">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C74" s="36"/>
       <c r="D74" s="36"/>
       <c r="E74" s="36"/>
       <c r="F74" s="37"/>
     </row>
-    <row r="75" spans="3:6">
+    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C75" s="36"/>
       <c r="D75" s="36"/>
       <c r="E75" s="36"/>
       <c r="F75" s="37"/>
     </row>
-    <row r="76" spans="3:6">
+    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C76" s="36"/>
       <c r="D76" s="36"/>
       <c r="E76" s="36"/>
       <c r="F76" s="37"/>
     </row>
-    <row r="77" spans="3:6">
+    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C77" s="36"/>
       <c r="D77" s="36"/>
       <c r="E77" s="36"/>
       <c r="F77" s="37"/>
     </row>
-    <row r="78" spans="3:6">
+    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C78" s="36"/>
       <c r="D78" s="36"/>
       <c r="E78" s="36"/>
@@ -3764,12 +3938,12 @@
       <selection sqref="A1:XFD81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5" style="17"/>
+    <col min="1" max="16384" width="11.42578125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" customFormat="1">
+    <row r="1" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1.7628000000000001E-2</v>
       </c>
@@ -3876,7 +4050,7 @@
         <v>-7.2519999999999998E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:35" customFormat="1">
+    <row r="2" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.6233999999999998E-2</v>
       </c>
@@ -3983,7 +4157,7 @@
         <v>-7.9830000000000005E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:35" customFormat="1">
+    <row r="3" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.5751000000000001E-2</v>
       </c>
@@ -4090,7 +4264,7 @@
         <v>-7.5119999999999996E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:35" customFormat="1">
+    <row r="4" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.6069E-2</v>
       </c>
@@ -4197,7 +4371,7 @@
         <v>-6.9760000000000004E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" customFormat="1">
+    <row r="5" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.1783E-2</v>
       </c>
@@ -4304,7 +4478,7 @@
         <v>-7.6280000000000002E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" customFormat="1">
+    <row r="6" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.0477999999999999E-2</v>
       </c>
@@ -4411,7 +4585,7 @@
         <v>-6.6010000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:35" customFormat="1">
+    <row r="7" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8.2439999999999996E-3</v>
       </c>
@@ -4518,7 +4692,7 @@
         <v>-5.9119999999999997E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:35" customFormat="1">
+    <row r="8" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8.3059999999999991E-3</v>
       </c>
@@ -4625,7 +4799,7 @@
         <v>-5.7159999999999997E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:35" customFormat="1">
+    <row r="9" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.7739999999999996E-3</v>
       </c>
@@ -4732,7 +4906,7 @@
         <v>-5.2129999999999998E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:35" customFormat="1">
+    <row r="10" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.4010000000000004E-3</v>
       </c>
@@ -4839,7 +5013,7 @@
         <v>-4.5580000000000004E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:35" customFormat="1">
+    <row r="11" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.0670000000000003E-3</v>
       </c>
@@ -4946,7 +5120,7 @@
         <v>-3.9480000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:35" customFormat="1">
+    <row r="12" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2.6800000000000001E-3</v>
       </c>
@@ -5053,7 +5227,7 @@
         <v>-3.3310000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" customFormat="1">
+    <row r="13" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2.0539999999999998E-3</v>
       </c>
@@ -5160,7 +5334,7 @@
         <v>-2.8830000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:35" customFormat="1">
+    <row r="14" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.2160000000000001E-3</v>
       </c>
@@ -5267,7 +5441,7 @@
         <v>-2.6900000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:35" customFormat="1">
+    <row r="15" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.2999999999999999E-4</v>
       </c>
@@ -5374,7 +5548,7 @@
         <v>-2.0699999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:35" customFormat="1">
+    <row r="16" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-4.37E-4</v>
       </c>
@@ -5481,7 +5655,7 @@
         <v>-1.8810000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:35" customFormat="1">
+    <row r="17" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-1.2049999999999999E-3</v>
       </c>
@@ -5588,7 +5762,7 @@
         <v>-1.4790000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:35" customFormat="1">
+    <row r="18" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-1.9170000000000001E-3</v>
       </c>
@@ -5695,7 +5869,7 @@
         <v>-1.3929999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:35" customFormat="1">
+    <row r="19" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-1.931E-3</v>
       </c>
@@ -5802,7 +5976,7 @@
         <v>-8.9499999999999996E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:35" customFormat="1">
+    <row r="20" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-2.2599999999999999E-3</v>
       </c>
@@ -5909,7 +6083,7 @@
         <v>-8.2200000000000003E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:35" customFormat="1">
+    <row r="21" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-2.5739999999999999E-3</v>
       </c>
@@ -6016,7 +6190,7 @@
         <v>-5.2999999999999998E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:35" customFormat="1">
+    <row r="22" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-2.6020000000000001E-3</v>
       </c>
@@ -6123,7 +6297,7 @@
         <v>-2.5799999999999998E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:35" customFormat="1">
+    <row r="23" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-2.702E-3</v>
       </c>
@@ -6230,7 +6404,7 @@
         <v>-2.2900000000000001E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:35" customFormat="1">
+    <row r="24" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-2.9919999999999999E-3</v>
       </c>
@@ -6337,7 +6511,7 @@
         <v>-3.3000000000000003E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:35" customFormat="1">
+    <row r="25" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-2.9719999999999998E-3</v>
       </c>
@@ -6444,7 +6618,7 @@
         <v>6.3E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:35" customFormat="1">
+    <row r="26" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-3.3040000000000001E-3</v>
       </c>
@@ -6551,7 +6725,7 @@
         <v>1.2899999999999999E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:35" customFormat="1">
+    <row r="27" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-3.4139999999999999E-3</v>
       </c>
@@ -6658,7 +6832,7 @@
         <v>2.5799999999999998E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:35" customFormat="1">
+    <row r="28" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-3.2989999999999998E-3</v>
       </c>
@@ -6765,7 +6939,7 @@
         <v>3.5100000000000002E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:35" customFormat="1">
+    <row r="29" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-3.362E-3</v>
       </c>
@@ -6872,7 +7046,7 @@
         <v>3.6900000000000002E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:35" customFormat="1">
+    <row r="30" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-3.467E-3</v>
       </c>
@@ -6979,7 +7153,7 @@
         <v>5.2099999999999998E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:35" customFormat="1">
+    <row r="31" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-3.519E-3</v>
       </c>
@@ -7086,7 +7260,7 @@
         <v>5.4299999999999997E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:35" customFormat="1">
+    <row r="32" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-3.588E-3</v>
       </c>
@@ -7193,7 +7367,7 @@
         <v>5.8200000000000005E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:35" customFormat="1">
+    <row r="33" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-3.5530000000000002E-3</v>
       </c>
@@ -7300,7 +7474,7 @@
         <v>6.4000000000000005E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:35" customFormat="1">
+    <row r="34" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-3.2499999999999999E-3</v>
       </c>
@@ -7407,7 +7581,7 @@
         <v>6.9499999999999998E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:35" customFormat="1">
+    <row r="35" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-3.4220000000000001E-3</v>
       </c>
@@ -7514,7 +7688,7 @@
         <v>6.9899999999999997E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:35" customFormat="1">
+    <row r="36" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>-3.4870000000000001E-3</v>
       </c>
@@ -7621,7 +7795,7 @@
         <v>7.7499999999999997E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:35" customFormat="1">
+    <row r="37" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>-3.738E-3</v>
       </c>
@@ -7728,7 +7902,7 @@
         <v>7.3899999999999997E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:35" customFormat="1">
+    <row r="38" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-3.7669999999999999E-3</v>
       </c>
@@ -7835,7 +8009,7 @@
         <v>6.4999999999999997E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:35" customFormat="1">
+    <row r="39" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-3.9060000000000002E-3</v>
       </c>
@@ -7942,7 +8116,7 @@
         <v>6.7599999999999995E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:35" customFormat="1">
+    <row r="40" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-3.8419999999999999E-3</v>
       </c>
@@ -8049,7 +8223,7 @@
         <v>7.2300000000000001E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:35" customFormat="1">
+    <row r="41" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-3.9389999999999998E-3</v>
       </c>
@@ -8156,7 +8330,7 @@
         <v>7.5100000000000004E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:35" customFormat="1">
+    <row r="42" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-4.1809999999999998E-3</v>
       </c>
@@ -8263,7 +8437,7 @@
         <v>5.8399999999999999E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:35" customFormat="1">
+    <row r="43" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-3.8500000000000001E-3</v>
       </c>
@@ -8370,7 +8544,7 @@
         <v>6.5600000000000001E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:35" customFormat="1">
+    <row r="44" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-3.8479999999999999E-3</v>
       </c>
@@ -8477,7 +8651,7 @@
         <v>5.8799999999999998E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:35" customFormat="1">
+    <row r="45" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-3.6640000000000002E-3</v>
       </c>
@@ -8584,7 +8758,7 @@
         <v>6.4700000000000001E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:35" customFormat="1">
+    <row r="46" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-3.6519999999999999E-3</v>
       </c>
@@ -8691,7 +8865,7 @@
         <v>6.7699999999999998E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:35" customFormat="1">
+    <row r="47" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-3.702E-3</v>
       </c>
@@ -8798,7 +8972,7 @@
         <v>6.7100000000000005E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:35" customFormat="1">
+    <row r="48" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-3.5850000000000001E-3</v>
       </c>
@@ -8905,7 +9079,7 @@
         <v>7.3999999999999999E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:35" customFormat="1">
+    <row r="49" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-3.7320000000000001E-3</v>
       </c>
@@ -9012,7 +9186,7 @@
         <v>6.9399999999999996E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:35" customFormat="1">
+    <row r="50" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-3.6740000000000002E-3</v>
       </c>
@@ -9119,7 +9293,7 @@
         <v>7.1400000000000001E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:35" customFormat="1">
+    <row r="51" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-3.7439999999999999E-3</v>
       </c>
@@ -9226,7 +9400,7 @@
         <v>7.2000000000000005E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:35" customFormat="1">
+    <row r="52" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-3.7950000000000002E-3</v>
       </c>
@@ -9333,7 +9507,7 @@
         <v>7.2000000000000005E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:35" customFormat="1">
+    <row r="53" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-3.7369999999999999E-3</v>
       </c>
@@ -9440,7 +9614,7 @@
         <v>7.1900000000000002E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:35" customFormat="1">
+    <row r="54" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-3.823E-3</v>
       </c>
@@ -9547,7 +9721,7 @@
         <v>6.8300000000000001E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:35" customFormat="1">
+    <row r="55" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-3.8769999999999998E-3</v>
       </c>
@@ -9654,7 +9828,7 @@
         <v>6.3100000000000005E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:35" customFormat="1">
+    <row r="56" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-4.0730000000000002E-3</v>
       </c>
@@ -9761,7 +9935,7 @@
         <v>6.3400000000000001E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:35" customFormat="1">
+    <row r="57" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-4.1370000000000001E-3</v>
       </c>
@@ -9868,7 +10042,7 @@
         <v>6.7699999999999998E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:35" customFormat="1">
+    <row r="58" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-4.13E-3</v>
       </c>
@@ -9975,7 +10149,7 @@
         <v>7.2199999999999999E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:35" customFormat="1">
+    <row r="59" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-4.1450000000000002E-3</v>
       </c>
@@ -10082,7 +10256,7 @@
         <v>6.7299999999999999E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:35" customFormat="1">
+    <row r="60" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-4.0730000000000002E-3</v>
       </c>
@@ -10189,7 +10363,7 @@
         <v>6.5499999999999998E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:35" customFormat="1">
+    <row r="61" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-4.0159999999999996E-3</v>
       </c>
@@ -10296,7 +10470,7 @@
         <v>6.7500000000000004E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:35" customFormat="1">
+    <row r="62" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-4.0080000000000003E-3</v>
       </c>
@@ -10403,7 +10577,7 @@
         <v>7.0699999999999995E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:35" customFormat="1">
+    <row r="63" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-3.9890000000000004E-3</v>
       </c>
@@ -10510,7 +10684,7 @@
         <v>7.1500000000000003E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:35" customFormat="1">
+    <row r="64" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-3.7750000000000001E-3</v>
       </c>
@@ -10617,7 +10791,7 @@
         <v>6.2799999999999998E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:35" customFormat="1">
+    <row r="65" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-3.6059999999999998E-3</v>
       </c>
@@ -10724,7 +10898,7 @@
         <v>6.6E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:35" customFormat="1">
+    <row r="66" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-3.3219999999999999E-3</v>
       </c>
@@ -10831,7 +11005,7 @@
         <v>5.9000000000000003E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:35" customFormat="1">
+    <row r="67" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-3.2629999999999998E-3</v>
       </c>
@@ -10938,7 +11112,7 @@
         <v>5.2700000000000002E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:35" customFormat="1">
+    <row r="68" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-3.114E-3</v>
       </c>
@@ -11045,7 +11219,7 @@
         <v>5.13E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:35" customFormat="1">
+    <row r="69" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-2.9380000000000001E-3</v>
       </c>
@@ -11152,7 +11326,7 @@
         <v>4.4900000000000002E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:35" customFormat="1">
+    <row r="70" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-2.8509999999999998E-3</v>
       </c>
@@ -11259,7 +11433,7 @@
         <v>4.4999999999999999E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:35" customFormat="1">
+    <row r="71" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-2.6589999999999999E-3</v>
       </c>
@@ -11366,7 +11540,7 @@
         <v>3.7100000000000002E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:35" customFormat="1">
+    <row r="72" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-2.5360000000000001E-3</v>
       </c>
@@ -11473,7 +11647,7 @@
         <v>4.6700000000000002E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:35" customFormat="1">
+    <row r="73" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-2.5149999999999999E-3</v>
       </c>
@@ -11580,7 +11754,7 @@
         <v>4.2499999999999998E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:35" customFormat="1">
+    <row r="74" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-2.7880000000000001E-3</v>
       </c>
@@ -11687,7 +11861,7 @@
         <v>4.7899999999999999E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:35" customFormat="1">
+    <row r="75" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-3.0019999999999999E-3</v>
       </c>
@@ -11794,7 +11968,7 @@
         <v>4.44E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:35" customFormat="1">
+    <row r="76" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-2.99E-3</v>
       </c>
@@ -11901,7 +12075,7 @@
         <v>4.6000000000000001E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:35" customFormat="1">
+    <row r="77" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-3.0990000000000002E-3</v>
       </c>
@@ -12008,7 +12182,7 @@
         <v>5.1099999999999995E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:35" customFormat="1">
+    <row r="78" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-3.0620000000000001E-3</v>
       </c>
@@ -12115,7 +12289,7 @@
         <v>4.7100000000000001E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:35" customFormat="1">
+    <row r="79" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-3.1870000000000002E-3</v>
       </c>
@@ -12222,7 +12396,7 @@
         <v>5.6400000000000005E-4</v>
       </c>
     </row>
-    <row r="80" spans="1:35" customFormat="1">
+    <row r="80" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-3.1640000000000001E-3</v>
       </c>
@@ -12329,7 +12503,7 @@
         <v>5.2999999999999998E-4</v>
       </c>
     </row>
-    <row r="81" customFormat="1"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -12349,12 +12523,12 @@
       <selection sqref="A1:XFD171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5" style="17"/>
+    <col min="1" max="16384" width="11.42578125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" customFormat="1">
+    <row r="1" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1.6018000000000001E-2</v>
       </c>
@@ -12461,7 +12635,7 @@
         <v>-1.3762E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:35" customFormat="1">
+    <row r="2" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6.7330000000000003E-3</v>
       </c>
@@ -12568,7 +12742,7 @@
         <v>-1.0474000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:35" customFormat="1">
+    <row r="3" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.9940000000000002E-3</v>
       </c>
@@ -12675,7 +12849,7 @@
         <v>-7.9799999999999992E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:35" customFormat="1">
+    <row r="4" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.8099999999999999E-4</v>
       </c>
@@ -12782,7 +12956,7 @@
         <v>-6.3499999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" customFormat="1">
+    <row r="5" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-4.0509999999999999E-3</v>
       </c>
@@ -12889,7 +13063,7 @@
         <v>-5.3239999999999997E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" customFormat="1">
+    <row r="6" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-4.5399999999999998E-3</v>
       </c>
@@ -12996,7 +13170,7 @@
         <v>-4.4149999999999997E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:35" customFormat="1">
+    <row r="7" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-7.2909999999999997E-3</v>
       </c>
@@ -13103,7 +13277,7 @@
         <v>-3.032E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:35" customFormat="1">
+    <row r="8" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-7.77E-3</v>
       </c>
@@ -13210,7 +13384,7 @@
         <v>-2.3340000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:35" customFormat="1">
+    <row r="9" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-7.8899999999999994E-3</v>
       </c>
@@ -13317,7 +13491,7 @@
         <v>-1.3290000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:35" customFormat="1">
+    <row r="10" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-9.8809999999999992E-3</v>
       </c>
@@ -13424,7 +13598,7 @@
         <v>-1.121E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:35" customFormat="1">
+    <row r="11" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-9.2359999999999994E-3</v>
       </c>
@@ -13531,7 +13705,7 @@
         <v>-5.4799999999999998E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:35" customFormat="1">
+    <row r="12" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-1.0222999999999999E-2</v>
       </c>
@@ -13638,7 +13812,7 @@
         <v>-3.21E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:35" customFormat="1">
+    <row r="13" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-1.0735E-2</v>
       </c>
@@ -13745,7 +13919,7 @@
         <v>-7.6000000000000004E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:35" customFormat="1">
+    <row r="14" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-0.01</v>
       </c>
@@ -13852,7 +14026,7 @@
         <v>2.8499999999999999E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:35" customFormat="1">
+    <row r="15" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-9.9179999999999997E-3</v>
       </c>
@@ -13959,7 +14133,7 @@
         <v>3.3399999999999999E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:35" customFormat="1">
+    <row r="16" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-9.5820000000000002E-3</v>
       </c>
@@ -14066,7 +14240,7 @@
         <v>7.0100000000000002E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:35" customFormat="1">
+    <row r="17" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-9.6159999999999995E-3</v>
       </c>
@@ -14173,7 +14347,7 @@
         <v>6.2600000000000004E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:35" customFormat="1">
+    <row r="18" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-8.7580000000000002E-3</v>
       </c>
@@ -14280,7 +14454,7 @@
         <v>9.1E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:35" customFormat="1">
+    <row r="19" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-8.7930000000000005E-3</v>
       </c>
@@ -14387,7 +14561,7 @@
         <v>7.7200000000000001E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:35" customFormat="1">
+    <row r="20" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-8.5979999999999997E-3</v>
       </c>
@@ -14494,7 +14668,7 @@
         <v>9.3000000000000005E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:35" customFormat="1">
+    <row r="21" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-8.2480000000000001E-3</v>
       </c>
@@ -14601,7 +14775,7 @@
         <v>8.7799999999999998E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:35" customFormat="1">
+    <row r="22" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-8.0529999999999994E-3</v>
       </c>
@@ -14708,7 +14882,7 @@
         <v>1.073E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:35" customFormat="1">
+    <row r="23" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-7.9729999999999992E-3</v>
       </c>
@@ -14815,7 +14989,7 @@
         <v>8.7699999999999996E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:35" customFormat="1">
+    <row r="24" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-6.881E-3</v>
       </c>
@@ -14922,7 +15096,7 @@
         <v>1.232E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:35" customFormat="1">
+    <row r="25" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-7.2509999999999996E-3</v>
       </c>
@@ -15029,7 +15203,7 @@
         <v>1.0319999999999999E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:35" customFormat="1">
+    <row r="26" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-6.9340000000000001E-3</v>
       </c>
@@ -15136,7 +15310,7 @@
         <v>1.1230000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:35" customFormat="1">
+    <row r="27" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-6.339E-3</v>
       </c>
@@ -15243,7 +15417,7 @@
         <v>1.152E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:35" customFormat="1">
+    <row r="28" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-6.7499999999999999E-3</v>
       </c>
@@ -15350,7 +15524,7 @@
         <v>1.0889999999999999E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:35" customFormat="1">
+    <row r="29" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-5.9880000000000003E-3</v>
       </c>
@@ -15457,7 +15631,7 @@
         <v>1.183E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:35" customFormat="1">
+    <row r="30" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-5.6340000000000001E-3</v>
       </c>
@@ -15564,7 +15738,7 @@
         <v>1.219E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:35" customFormat="1">
+    <row r="31" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-6.0439999999999999E-3</v>
       </c>
@@ -15671,7 +15845,7 @@
         <v>1.183E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:35" customFormat="1">
+    <row r="32" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-5.3660000000000001E-3</v>
       </c>
@@ -15778,7 +15952,7 @@
         <v>1.175E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:35" customFormat="1">
+    <row r="33" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-5.3439999999999998E-3</v>
       </c>
@@ -15885,7 +16059,7 @@
         <v>1.266E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:35" customFormat="1">
+    <row r="34" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-5.2919999999999998E-3</v>
       </c>
@@ -15992,7 +16166,7 @@
         <v>1.2049999999999999E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:35" customFormat="1">
+    <row r="35" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-5.0159999999999996E-3</v>
       </c>
@@ -16099,7 +16273,7 @@
         <v>1.103E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35" customFormat="1">
+    <row r="36" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>-5.5339999999999999E-3</v>
       </c>
@@ -16206,7 +16380,7 @@
         <v>1.178E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:35" customFormat="1">
+    <row r="37" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>-5.718E-3</v>
       </c>
@@ -16313,7 +16487,7 @@
         <v>1.021E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:35" customFormat="1">
+    <row r="38" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-5.228E-3</v>
       </c>
@@ -16420,7 +16594,7 @@
         <v>1.0629999999999999E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:35" customFormat="1">
+    <row r="39" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-5.3730000000000002E-3</v>
       </c>
@@ -16527,7 +16701,7 @@
         <v>9.9700000000000006E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:35" customFormat="1">
+    <row r="40" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-5.1070000000000004E-3</v>
       </c>
@@ -16634,7 +16808,7 @@
         <v>9.3999999999999997E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:35" customFormat="1">
+    <row r="41" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-5.0109999999999998E-3</v>
       </c>
@@ -16741,7 +16915,7 @@
         <v>8.8400000000000002E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:35" customFormat="1">
+    <row r="42" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-6.1219999999999998E-3</v>
       </c>
@@ -16848,7 +17022,7 @@
         <v>4.44E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:35" customFormat="1">
+    <row r="43" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-5.8999999999999999E-3</v>
       </c>
@@ -16955,7 +17129,7 @@
         <v>4.8500000000000003E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:35" customFormat="1">
+    <row r="44" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-6.0340000000000003E-3</v>
       </c>
@@ -17062,7 +17236,7 @@
         <v>5.1900000000000004E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:35" customFormat="1">
+    <row r="45" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-5.8370000000000002E-3</v>
       </c>
@@ -17169,7 +17343,7 @@
         <v>5.4900000000000001E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:35" customFormat="1">
+    <row r="46" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-5.4539999999999996E-3</v>
       </c>
@@ -17276,7 +17450,7 @@
         <v>6.4599999999999998E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:35" customFormat="1">
+    <row r="47" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-5.4359999999999999E-3</v>
       </c>
@@ -17383,7 +17557,7 @@
         <v>6.9499999999999998E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:35" customFormat="1">
+    <row r="48" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-5.0990000000000002E-3</v>
       </c>
@@ -17490,7 +17664,7 @@
         <v>7.6999999999999996E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:35" customFormat="1">
+    <row r="49" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-4.8640000000000003E-3</v>
       </c>
@@ -17597,7 +17771,7 @@
         <v>8.1300000000000003E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:35" customFormat="1">
+    <row r="50" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-4.712E-3</v>
       </c>
@@ -17704,7 +17878,7 @@
         <v>8.4900000000000004E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:35" customFormat="1">
+    <row r="51" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-4.2810000000000001E-3</v>
       </c>
@@ -17811,7 +17985,7 @@
         <v>9.3300000000000002E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:35" customFormat="1">
+    <row r="52" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-4.3200000000000001E-3</v>
       </c>
@@ -17918,7 +18092,7 @@
         <v>9.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:35" customFormat="1">
+    <row r="53" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-3.8809999999999999E-3</v>
       </c>
@@ -18025,7 +18199,7 @@
         <v>9.7300000000000002E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:35" customFormat="1">
+    <row r="54" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-3.4489999999999998E-3</v>
       </c>
@@ -18132,7 +18306,7 @@
         <v>9.8700000000000003E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:35" customFormat="1">
+    <row r="55" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-3.137E-3</v>
       </c>
@@ -18239,7 +18413,7 @@
         <v>1.008E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:35" customFormat="1">
+    <row r="56" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-3.0400000000000002E-3</v>
       </c>
@@ -18346,7 +18520,7 @@
         <v>8.8500000000000004E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:35" customFormat="1">
+    <row r="57" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-3.0929999999999998E-3</v>
       </c>
@@ -18453,7 +18627,7 @@
         <v>9.5500000000000001E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:35" customFormat="1">
+    <row r="58" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-3.2560000000000002E-3</v>
       </c>
@@ -18560,7 +18734,7 @@
         <v>8.8099999999999995E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:35" customFormat="1">
+    <row r="59" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-3.0360000000000001E-3</v>
       </c>
@@ -18667,7 +18841,7 @@
         <v>8.2299999999999995E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:35" customFormat="1">
+    <row r="60" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-3.1819999999999999E-3</v>
       </c>
@@ -18774,7 +18948,7 @@
         <v>8.7100000000000003E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:35" customFormat="1">
+    <row r="61" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-3.0460000000000001E-3</v>
       </c>
@@ -18881,7 +19055,7 @@
         <v>8.1700000000000002E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:35" customFormat="1">
+    <row r="62" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-2.8700000000000002E-3</v>
       </c>
@@ -18988,7 +19162,7 @@
         <v>8.0199999999999998E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:35" customFormat="1">
+    <row r="63" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-3.1229999999999999E-3</v>
       </c>
@@ -19095,7 +19269,7 @@
         <v>7.6800000000000002E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:35" customFormat="1">
+    <row r="64" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-2.9290000000000002E-3</v>
       </c>
@@ -19202,7 +19376,7 @@
         <v>6.7900000000000002E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:35" customFormat="1">
+    <row r="65" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-3.153E-3</v>
       </c>
@@ -19309,7 +19483,7 @@
         <v>7.4100000000000001E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:35" customFormat="1">
+    <row r="66" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-2.99E-3</v>
       </c>
@@ -19416,7 +19590,7 @@
         <v>6.8000000000000005E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:35" customFormat="1">
+    <row r="67" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-2.6809999999999998E-3</v>
       </c>
@@ -19523,7 +19697,7 @@
         <v>5.9100000000000005E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:35" customFormat="1">
+    <row r="68" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-2.6210000000000001E-3</v>
       </c>
@@ -19630,7 +19804,7 @@
         <v>6.2399999999999999E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:35" customFormat="1">
+    <row r="69" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-2.4329999999999998E-3</v>
       </c>
@@ -19737,7 +19911,7 @@
         <v>5.4100000000000003E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:35" customFormat="1">
+    <row r="70" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-2.2139999999999998E-3</v>
       </c>
@@ -19844,7 +20018,7 @@
         <v>4.8000000000000001E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:35" customFormat="1">
+    <row r="71" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-2.5929999999999998E-3</v>
       </c>
@@ -19951,7 +20125,7 @@
         <v>4.66E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:35" customFormat="1">
+    <row r="72" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-2.5769999999999999E-3</v>
       </c>
@@ -20058,7 +20232,7 @@
         <v>4.84E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:35" customFormat="1">
+    <row r="73" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-2.6159999999999998E-3</v>
       </c>
@@ -20165,7 +20339,7 @@
         <v>4.35E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:35" customFormat="1">
+    <row r="74" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-2.748E-3</v>
       </c>
@@ -20272,7 +20446,7 @@
         <v>5.0699999999999996E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:35" customFormat="1">
+    <row r="75" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-2.7959999999999999E-3</v>
       </c>
@@ -20379,7 +20553,7 @@
         <v>4.4999999999999999E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:35" customFormat="1">
+    <row r="76" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-3.0330000000000001E-3</v>
       </c>
@@ -20486,7 +20660,7 @@
         <v>3.3300000000000002E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:35" customFormat="1">
+    <row r="77" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-3.4020000000000001E-3</v>
       </c>
@@ -20593,7 +20767,7 @@
         <v>3.2200000000000002E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:35" customFormat="1">
+    <row r="78" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-3.434E-3</v>
       </c>
@@ -20700,7 +20874,7 @@
         <v>2.1699999999999999E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:35" customFormat="1">
+    <row r="79" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-3.9129999999999998E-3</v>
       </c>
@@ -20807,7 +20981,7 @@
         <v>3.9599999999999998E-4</v>
       </c>
     </row>
-    <row r="80" spans="1:35" customFormat="1">
+    <row r="80" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-4.6620000000000003E-3</v>
       </c>
@@ -20914,97 +21088,97 @@
         <v>-6.8999999999999997E-5</v>
       </c>
     </row>
-    <row r="81" customFormat="1"/>
-    <row r="82" customFormat="1"/>
-    <row r="83" customFormat="1"/>
-    <row r="84" customFormat="1"/>
-    <row r="85" customFormat="1"/>
-    <row r="86" customFormat="1"/>
-    <row r="87" customFormat="1"/>
-    <row r="88" customFormat="1"/>
-    <row r="89" customFormat="1"/>
-    <row r="90" customFormat="1"/>
-    <row r="91" customFormat="1"/>
-    <row r="92" customFormat="1"/>
-    <row r="93" customFormat="1"/>
-    <row r="94" customFormat="1"/>
-    <row r="95" customFormat="1"/>
-    <row r="96" customFormat="1"/>
-    <row r="97" customFormat="1"/>
-    <row r="98" customFormat="1"/>
-    <row r="99" customFormat="1"/>
-    <row r="100" customFormat="1"/>
-    <row r="101" customFormat="1"/>
-    <row r="102" customFormat="1"/>
-    <row r="103" customFormat="1"/>
-    <row r="104" customFormat="1"/>
-    <row r="105" customFormat="1"/>
-    <row r="106" customFormat="1"/>
-    <row r="107" customFormat="1"/>
-    <row r="108" customFormat="1"/>
-    <row r="109" customFormat="1"/>
-    <row r="110" customFormat="1"/>
-    <row r="111" customFormat="1"/>
-    <row r="112" customFormat="1"/>
-    <row r="113" customFormat="1"/>
-    <row r="114" customFormat="1"/>
-    <row r="115" customFormat="1"/>
-    <row r="116" customFormat="1"/>
-    <row r="117" customFormat="1"/>
-    <row r="118" customFormat="1"/>
-    <row r="119" customFormat="1"/>
-    <row r="120" customFormat="1"/>
-    <row r="121" customFormat="1"/>
-    <row r="122" customFormat="1"/>
-    <row r="123" customFormat="1"/>
-    <row r="124" customFormat="1"/>
-    <row r="125" customFormat="1"/>
-    <row r="126" customFormat="1"/>
-    <row r="127" customFormat="1"/>
-    <row r="128" customFormat="1"/>
-    <row r="129" customFormat="1"/>
-    <row r="130" customFormat="1"/>
-    <row r="131" customFormat="1"/>
-    <row r="132" customFormat="1"/>
-    <row r="133" customFormat="1"/>
-    <row r="134" customFormat="1"/>
-    <row r="135" customFormat="1"/>
-    <row r="136" customFormat="1"/>
-    <row r="137" customFormat="1"/>
-    <row r="138" customFormat="1"/>
-    <row r="139" customFormat="1"/>
-    <row r="140" customFormat="1"/>
-    <row r="141" customFormat="1"/>
-    <row r="142" customFormat="1"/>
-    <row r="143" customFormat="1"/>
-    <row r="144" customFormat="1"/>
-    <row r="145" customFormat="1"/>
-    <row r="146" customFormat="1"/>
-    <row r="147" customFormat="1"/>
-    <row r="148" customFormat="1"/>
-    <row r="149" customFormat="1"/>
-    <row r="150" customFormat="1"/>
-    <row r="151" customFormat="1"/>
-    <row r="152" customFormat="1"/>
-    <row r="153" customFormat="1"/>
-    <row r="154" customFormat="1"/>
-    <row r="155" customFormat="1"/>
-    <row r="156" customFormat="1"/>
-    <row r="157" customFormat="1"/>
-    <row r="158" customFormat="1"/>
-    <row r="159" customFormat="1"/>
-    <row r="160" customFormat="1"/>
-    <row r="161" customFormat="1"/>
-    <row r="162" customFormat="1"/>
-    <row r="163" customFormat="1"/>
-    <row r="164" customFormat="1"/>
-    <row r="165" customFormat="1"/>
-    <row r="166" customFormat="1"/>
-    <row r="167" customFormat="1"/>
-    <row r="168" customFormat="1"/>
-    <row r="169" customFormat="1"/>
-    <row r="170" customFormat="1"/>
-    <row r="171" customFormat="1"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="154" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="158" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="159" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="161" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="164" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="166" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="167" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="168" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="170" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="171" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>